<commit_message>
Various additions to DrawPoints
</commit_message>
<xml_diff>
--- a/MaxTranPatsJava/Analysis/FJvsMT.xlsx
+++ b/MaxTranPatsJava/Analysis/FJvsMT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanne/Repos/omnisia/MaxTranPatsJava/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B9627A-1781-9848-8769-79BC6C94A10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5A4BEC-2F25-0149-888E-79E260A1FFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27360" yWindow="500" windowWidth="27360" windowHeight="21900" xr2:uid="{43F56DD3-E27F-E149-A1E7-C63A26642EBF}"/>
+    <workbookView xWindow="-31600" yWindow="500" windowWidth="31600" windowHeight="21900" xr2:uid="{43F56DD3-E27F-E149-A1E7-C63A26642EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>|D|</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>sqrt of num computations</t>
+  </si>
+  <si>
+    <t>Strato 127</t>
+  </si>
+  <si>
+    <t>Out of heap space error</t>
+  </si>
+  <si>
+    <t>Out of heap space</t>
   </si>
 </sst>
 </file>
@@ -442,11 +451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290D561E-741C-EE44-B52E-5D40ADD54BC2}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="257" zoomScaleNormal="257" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,13 +463,14 @@
     <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +498,11 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -505,8 +518,11 @@
       <c r="E2">
         <v>11100</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>19884</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>100</v>
       </c>
@@ -522,8 +538,11 @@
       <c r="E3">
         <v>38328</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>56897</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
@@ -539,8 +558,11 @@
       <c r="E4">
         <v>37665</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>59294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>100</v>
       </c>
@@ -560,7 +582,7 @@
         <v>41507</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>100</v>
       </c>
@@ -583,7 +605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
@@ -603,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
@@ -620,7 +642,7 @@
         <v>29176</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
@@ -640,7 +662,7 @@
         <v>24393</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
@@ -662,8 +684,11 @@
       <c r="I10">
         <v>23350</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>49978</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -680,7 +705,7 @@
         <v>27211</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>100</v>
       </c>
@@ -697,7 +722,7 @@
         <v>32846</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
@@ -714,7 +739,7 @@
         <v>37065</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
@@ -731,7 +756,7 @@
         <v>37808</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>100</v>
       </c>
@@ -748,7 +773,7 @@
         <v>37225</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>100</v>
       </c>
@@ -765,7 +790,7 @@
         <v>36564</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>100</v>
       </c>
@@ -782,7 +807,7 @@
         <v>37398</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>100</v>
       </c>
@@ -799,7 +824,7 @@
         <v>36788</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>100</v>
       </c>
@@ -816,7 +841,7 @@
         <v>30579</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>100</v>
       </c>
@@ -833,7 +858,7 @@
         <v>30853</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>100</v>
       </c>
@@ -849,8 +874,11 @@
       <c r="E21">
         <v>28217</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>59728</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>100</v>
       </c>
@@ -867,7 +895,7 @@
         <v>28438</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>100</v>
       </c>
@@ -884,7 +912,7 @@
         <v>29913</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>100</v>
       </c>
@@ -900,11 +928,11 @@
       <c r="E24">
         <v>28291</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>100</v>
       </c>
@@ -919,6 +947,117 @@
       </c>
       <c r="E25">
         <v>29308</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>100</v>
+      </c>
+      <c r="B26">
+        <v>100000</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>36117</v>
+      </c>
+      <c r="H26">
+        <v>36424</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>150</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>61840</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>150</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>142366</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>200</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29">
+        <v>1105204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>200</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30">
+        <v>379378</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>250</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>